<commit_message>
Updated to the latest version
</commit_message>
<xml_diff>
--- a/heat-dist-results.xlsx
+++ b/heat-dist-results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaming PC\Downloads\heat-distribution-main\heat-distribution-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{053E2B7A-4F43-8042-9132-2E71C54F8EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025C5667-0952-4A61-AFEC-4FD6AF8F5CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10740" yWindow="-24400" windowWidth="28040" windowHeight="17440" xr2:uid="{7604C183-4522-3844-BE9D-3DB05E68BAB2}"/>
+    <workbookView xWindow="-31635" yWindow="2895" windowWidth="28800" windowHeight="15435" xr2:uid="{7604C183-4522-3844-BE9D-3DB05E68BAB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="25">
   <si>
     <t>št. Iteracij</t>
   </si>
@@ -66,12 +57,6 @@
     <t>1000x1000</t>
   </si>
   <si>
-    <t>10000 iteracij, spreminjamo velikost kvadratne matrike NxN.  Pri OMP uporabi 32 jeder oziroma kolikor je največ možno, pri MPI 32 ali 64.</t>
-  </si>
-  <si>
-    <t>1000x1000 matrika, spreminjamo št. Iteracij. Pri OMP uporabi 32 jeder oziroma kolikor je največ možno, pri MPI 32 ali 64.</t>
-  </si>
-  <si>
     <t>10000 iteracij, 10^6 elementov v matriki, spreminjamo razmerje med višino in širino matrike.  Pri OMP uporabi 32 jeder oziroma kolikor je največ možno, pri MPI 32 ali 64.</t>
   </si>
   <si>
@@ -106,6 +91,15 @@
   </si>
   <si>
     <t>OpenMP, 10000 iteracij, 1000x1000 matrika, spreminjamo število niti.</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>1000x1000 matrika, spreminjamo št. Iteracij. Pri OMP uporabi 32 jeder oziroma kolikor je največ možno, pri MPI 32 na dveh nodih.</t>
+  </si>
+  <si>
+    <t>10000 iteracij, spreminjamo velikost kvadratne matrike NxN.  Pri OMP uporabi 32 jeder oziroma kolikor je največ možno, pri MPI 32 na dveh nodih.</t>
   </si>
 </sst>
 </file>
@@ -232,15 +226,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,39 +551,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60E9CCC9-2FE9-B644-98E2-070603DD8D20}">
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J60" sqref="J60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
@@ -615,7 +609,7 @@
       </c>
       <c r="O6" s="3"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>0</v>
       </c>
@@ -651,7 +645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="4">
         <v>10000</v>
@@ -663,12 +657,16 @@
       <c r="E8" s="5">
         <v>10000</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="12">
+        <v>10.8</v>
+      </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5">
         <v>10000</v>
       </c>
-      <c r="I8" s="5"/>
+      <c r="I8" s="5">
+        <v>8.3000000000000007</v>
+      </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5">
         <v>10000</v>
@@ -684,7 +682,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <v>1000</v>
       </c>
@@ -695,12 +693,16 @@
       <c r="E9" s="5">
         <v>1000</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="12">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5">
         <v>1000</v>
       </c>
-      <c r="I9" s="5"/>
+      <c r="I9" s="5">
+        <v>1.2</v>
+      </c>
       <c r="J9" s="5"/>
       <c r="K9" s="5">
         <v>1000</v>
@@ -716,7 +718,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <v>100</v>
       </c>
@@ -727,12 +729,16 @@
       <c r="E10" s="5">
         <v>100</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="12">
+        <v>0.48</v>
+      </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5">
         <v>100</v>
       </c>
-      <c r="I10" s="5"/>
+      <c r="I10" s="5">
+        <v>0.44</v>
+      </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5">
         <v>100</v>
@@ -748,7 +754,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>10</v>
       </c>
@@ -759,12 +765,16 @@
       <c r="E11" s="8">
         <v>10</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="8">
+        <v>0.05</v>
+      </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8">
         <v>10</v>
       </c>
-      <c r="I11" s="8"/>
+      <c r="I11" s="8">
+        <v>0.38</v>
+      </c>
       <c r="J11" s="8"/>
       <c r="K11" s="8">
         <v>10</v>
@@ -780,26 +790,26 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="B14" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B14" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="1" t="s">
         <v>2</v>
@@ -826,7 +836,7 @@
       </c>
       <c r="O15" s="3"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
@@ -863,139 +873,155 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
-      <c r="B17" s="11">
+      <c r="B17" s="10">
         <v>1000</v>
       </c>
       <c r="C17" s="5">
         <v>263.11</v>
       </c>
       <c r="D17" s="5"/>
-      <c r="E17" s="13">
+      <c r="E17" s="11">
         <v>1000</v>
       </c>
-      <c r="F17" s="5"/>
+      <c r="F17" s="12">
+        <v>10.7</v>
+      </c>
       <c r="G17" s="5"/>
-      <c r="H17" s="13">
+      <c r="H17" s="11">
         <v>1000</v>
       </c>
-      <c r="I17" s="5"/>
+      <c r="I17" s="5">
+        <v>8.1</v>
+      </c>
       <c r="J17" s="5"/>
-      <c r="K17" s="13">
+      <c r="K17" s="11">
         <v>1000</v>
       </c>
       <c r="L17" s="5">
         <v>4.55</v>
       </c>
       <c r="M17" s="5"/>
-      <c r="N17" s="13">
+      <c r="N17" s="11">
         <v>1000</v>
       </c>
       <c r="O17" s="6">
         <v>2.58</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
-      <c r="B18" s="11">
+      <c r="B18" s="10">
         <v>750</v>
       </c>
       <c r="C18" s="5">
         <v>128.5</v>
       </c>
       <c r="D18" s="5"/>
-      <c r="E18" s="13">
+      <c r="E18" s="11">
         <v>750</v>
       </c>
-      <c r="F18" s="5"/>
+      <c r="F18" s="12">
+        <v>6.2</v>
+      </c>
       <c r="G18" s="5"/>
-      <c r="H18" s="13">
+      <c r="H18" s="11">
         <v>750</v>
       </c>
-      <c r="I18" s="5"/>
+      <c r="I18" s="5">
+        <v>4.0999999999999996</v>
+      </c>
       <c r="J18" s="5"/>
-      <c r="K18" s="13">
+      <c r="K18" s="11">
         <v>750</v>
       </c>
       <c r="L18" s="5">
         <v>2.6</v>
       </c>
       <c r="M18" s="5"/>
-      <c r="N18" s="13">
+      <c r="N18" s="11">
         <v>750</v>
       </c>
       <c r="O18" s="6">
         <v>1.5</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
-      <c r="B19" s="11">
+      <c r="B19" s="10">
         <v>500</v>
       </c>
       <c r="C19" s="5">
         <v>50.68</v>
       </c>
       <c r="D19" s="5"/>
-      <c r="E19" s="13">
+      <c r="E19" s="11">
         <v>500</v>
       </c>
-      <c r="F19" s="5"/>
+      <c r="F19" s="12">
+        <v>2.8</v>
+      </c>
       <c r="G19" s="5"/>
-      <c r="H19" s="13">
+      <c r="H19" s="11">
         <v>500</v>
       </c>
-      <c r="I19" s="5"/>
+      <c r="I19" s="5">
+        <v>3.9</v>
+      </c>
       <c r="J19" s="5"/>
-      <c r="K19" s="13">
+      <c r="K19" s="11">
         <v>500</v>
       </c>
       <c r="L19" s="5">
         <v>1.22</v>
       </c>
       <c r="M19" s="5"/>
-      <c r="N19" s="13">
+      <c r="N19" s="11">
         <v>500</v>
       </c>
       <c r="O19" s="6">
         <v>0.73</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
-      <c r="B20" s="11">
+      <c r="B20" s="10">
         <v>250</v>
       </c>
       <c r="C20" s="5">
         <v>11.57</v>
       </c>
       <c r="D20" s="5"/>
-      <c r="E20" s="13">
+      <c r="E20" s="11">
         <v>250</v>
       </c>
-      <c r="F20" s="5"/>
+      <c r="F20" s="12">
+        <v>0.83</v>
+      </c>
       <c r="G20" s="5"/>
-      <c r="H20" s="13">
+      <c r="H20" s="11">
         <v>250</v>
       </c>
-      <c r="I20" s="5"/>
+      <c r="I20" s="12">
+        <v>2.75</v>
+      </c>
       <c r="J20" s="5"/>
-      <c r="K20" s="13">
+      <c r="K20" s="11">
         <v>250</v>
       </c>
-      <c r="L20" s="14">
+      <c r="L20" s="12">
         <v>0.37</v>
       </c>
       <c r="M20" s="5"/>
-      <c r="N20" s="13">
+      <c r="N20" s="11">
         <v>250</v>
       </c>
       <c r="O20" s="6">
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="7">
         <v>100</v>
@@ -1007,12 +1033,16 @@
       <c r="E21" s="8">
         <v>100</v>
       </c>
-      <c r="F21" s="8"/>
+      <c r="F21" s="8">
+        <v>0.34</v>
+      </c>
       <c r="G21" s="8"/>
       <c r="H21" s="8">
         <v>100</v>
       </c>
-      <c r="I21" s="8"/>
+      <c r="I21" s="8">
+        <v>1.6</v>
+      </c>
       <c r="J21" s="8"/>
       <c r="K21" s="8">
         <v>100</v>
@@ -1028,28 +1058,28 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B24" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
-      <c r="O24" s="12"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="17"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>2</v>
       </c>
@@ -1061,269 +1091,239 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="O25" s="3"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G26" s="5"/>
       <c r="H26" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>1</v>
       </c>
       <c r="J26" s="5"/>
       <c r="K26" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="L26" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="O26" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B27" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="L26" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B27" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C27" s="5">
         <v>263.11</v>
       </c>
       <c r="D27" s="5"/>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="5"/>
+      <c r="F27" s="5">
+        <v>10.7</v>
+      </c>
       <c r="G27" s="5"/>
-      <c r="H27" s="13" t="s">
+      <c r="H27" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I27" s="5"/>
+      <c r="I27" s="5">
+        <v>4.55</v>
+      </c>
       <c r="J27" s="5"/>
-      <c r="K27" s="13" t="s">
+      <c r="K27" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="L27" s="5">
-        <v>4.55</v>
-      </c>
-      <c r="M27" s="5"/>
-      <c r="N27" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="O27" s="6">
+      <c r="L27" s="6">
         <v>2.58</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B28" s="11" t="s">
-        <v>13</v>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B28" s="10" t="s">
+        <v>11</v>
       </c>
       <c r="C28" s="5">
         <v>227.45</v>
       </c>
       <c r="D28" s="5"/>
-      <c r="E28" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F28" s="5"/>
+      <c r="E28" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="5">
+        <v>10.9</v>
+      </c>
       <c r="G28" s="5"/>
-      <c r="H28" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I28" s="5"/>
+      <c r="H28" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28" s="5">
+        <v>4.55</v>
+      </c>
       <c r="J28" s="5"/>
-      <c r="K28" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="L28" s="5">
-        <v>4.55</v>
-      </c>
-      <c r="M28" s="5"/>
-      <c r="N28" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="O28" s="6">
+      <c r="K28" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L28" s="6">
         <v>2.59</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B29" s="11" t="s">
-        <v>14</v>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="C29" s="5">
         <v>220.34</v>
       </c>
       <c r="D29" s="5"/>
-      <c r="E29" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" s="5"/>
+      <c r="E29" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="5">
+        <v>11</v>
+      </c>
       <c r="G29" s="5"/>
-      <c r="H29" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I29" s="5"/>
+      <c r="H29" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I29" s="5">
+        <v>4.57</v>
+      </c>
       <c r="J29" s="5"/>
-      <c r="K29" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="L29" s="5">
-        <v>4.57</v>
-      </c>
-      <c r="M29" s="5"/>
-      <c r="N29" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="O29" s="6">
+      <c r="K29" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="L29" s="6">
         <v>2.6</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B30" s="11" t="s">
-        <v>15</v>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B30" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="C30" s="5">
         <v>210.85</v>
       </c>
       <c r="D30" s="5"/>
-      <c r="E30" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F30" s="5"/>
+      <c r="E30" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="12">
+        <v>13.7</v>
+      </c>
       <c r="G30" s="5"/>
-      <c r="H30" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I30" s="5"/>
+      <c r="H30" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I30" s="5">
+        <v>4.59</v>
+      </c>
       <c r="J30" s="5"/>
-      <c r="K30" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="L30" s="5">
-        <v>4.59</v>
-      </c>
-      <c r="M30" s="5"/>
-      <c r="N30" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="O30" s="6">
+      <c r="K30" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="L30" s="6">
         <v>2.7</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B31" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" s="14">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B31" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="12">
         <v>189.91</v>
       </c>
       <c r="D31" s="5"/>
-      <c r="E31" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F31" s="5"/>
+      <c r="E31" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" s="12">
+        <v>50</v>
+      </c>
       <c r="G31" s="5"/>
-      <c r="H31" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="I31" s="5"/>
+      <c r="H31" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" s="12">
+        <v>4.63</v>
+      </c>
       <c r="J31" s="5"/>
-      <c r="K31" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="L31" s="14">
-        <v>4.63</v>
-      </c>
-      <c r="M31" s="5"/>
-      <c r="N31" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="O31" s="6">
+      <c r="K31" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L31" s="6">
         <v>2.81</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B32" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C32" s="8">
         <v>165.88</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32" s="8"/>
+        <v>14</v>
+      </c>
+      <c r="F32" s="8">
+        <v>40</v>
+      </c>
       <c r="G32" s="8"/>
       <c r="H32" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I32" s="8"/>
+        <v>14</v>
+      </c>
+      <c r="I32" s="8">
+        <v>2.0699999999999998</v>
+      </c>
       <c r="J32" s="8"/>
       <c r="K32" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L32" s="8">
-        <v>2.0699999999999998</v>
-      </c>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="O32" s="9">
+        <v>14</v>
+      </c>
+      <c r="L32" s="9">
         <v>1.72</v>
       </c>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B35" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="12"/>
-      <c r="L35" s="12"/>
-      <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
-      <c r="O35" s="12"/>
-    </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B35" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="17"/>
+      <c r="O35" s="17"/>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>1</v>
@@ -1341,11 +1341,13 @@
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B37" s="11">
-        <v>1</v>
-      </c>
-      <c r="C37" s="6"/>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B37" s="10">
+        <v>1</v>
+      </c>
+      <c r="C37" s="6">
+        <v>282</v>
+      </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
@@ -1359,97 +1361,107 @@
       <c r="N37" s="5"/>
       <c r="O37" s="5"/>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B38" s="11">
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B38" s="10">
         <v>2</v>
       </c>
-      <c r="C38" s="6"/>
+      <c r="C38" s="6">
+        <v>152</v>
+      </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
-      <c r="H38" s="13"/>
+      <c r="H38" s="11"/>
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
-      <c r="K38" s="13"/>
+      <c r="K38" s="11"/>
       <c r="L38" s="5"/>
       <c r="M38" s="5"/>
-      <c r="N38" s="13"/>
+      <c r="N38" s="11"/>
       <c r="O38" s="5"/>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B39" s="11">
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B39" s="10">
         <v>4</v>
       </c>
-      <c r="C39" s="6"/>
+      <c r="C39" s="6">
+        <v>81</v>
+      </c>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
-      <c r="H39" s="13"/>
+      <c r="H39" s="11"/>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
-      <c r="K39" s="13"/>
+      <c r="K39" s="11"/>
       <c r="L39" s="5"/>
       <c r="M39" s="5"/>
-      <c r="N39" s="13"/>
+      <c r="N39" s="11"/>
       <c r="O39" s="5"/>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B40" s="11">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B40" s="10">
         <v>8</v>
       </c>
-      <c r="C40" s="6"/>
+      <c r="C40" s="6">
+        <v>39</v>
+      </c>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
-      <c r="H40" s="13"/>
+      <c r="H40" s="11"/>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
-      <c r="K40" s="13"/>
+      <c r="K40" s="11"/>
       <c r="L40" s="5"/>
       <c r="M40" s="5"/>
-      <c r="N40" s="13"/>
+      <c r="N40" s="11"/>
       <c r="O40" s="5"/>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B41" s="15">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B41" s="13">
         <v>16</v>
       </c>
-      <c r="C41" s="6"/>
+      <c r="C41" s="6">
+        <v>20.5</v>
+      </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
-      <c r="H41" s="13"/>
+      <c r="H41" s="11"/>
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
-      <c r="K41" s="13"/>
+      <c r="K41" s="11"/>
       <c r="L41" s="5"/>
       <c r="M41" s="5"/>
-      <c r="N41" s="13"/>
+      <c r="N41" s="11"/>
       <c r="O41" s="5"/>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B42" s="7">
         <v>32</v>
       </c>
-      <c r="C42" s="9"/>
+      <c r="C42" s="9">
+        <v>10.7</v>
+      </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
-      <c r="H42" s="16"/>
+      <c r="H42" s="14"/>
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
-      <c r="K42" s="16"/>
-      <c r="L42" s="14"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="12"/>
       <c r="M42" s="5"/>
-      <c r="N42" s="16"/>
+      <c r="N42" s="14"/>
       <c r="O42" s="5"/>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
@@ -1463,32 +1475,32 @@
       <c r="N43" s="5"/>
       <c r="O43" s="5"/>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B45" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="12"/>
-      <c r="K45" s="12"/>
-      <c r="L45" s="12"/>
-      <c r="M45" s="12"/>
-      <c r="N45" s="12"/>
-      <c r="O45" s="12"/>
-    </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B45" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="17"/>
+      <c r="J45" s="17"/>
+      <c r="K45" s="17"/>
+      <c r="L45" s="17"/>
+      <c r="M45" s="17"/>
+      <c r="N45" s="17"/>
+      <c r="O45" s="17"/>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="5"/>
@@ -1501,16 +1513,16 @@
       <c r="N46" s="5"/>
       <c r="O46" s="5"/>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>1</v>
@@ -1525,127 +1537,155 @@
       <c r="N47" s="5"/>
       <c r="O47" s="5"/>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B48" s="11">
-        <v>1</v>
-      </c>
-      <c r="C48" s="5"/>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B48" s="10">
+        <v>1</v>
+      </c>
+      <c r="C48" s="5">
+        <v>58</v>
+      </c>
       <c r="D48" s="5"/>
-      <c r="E48" s="13">
-        <v>1</v>
-      </c>
-      <c r="F48" s="6"/>
+      <c r="E48" s="11">
+        <v>1</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="G48" s="5"/>
-      <c r="H48" s="13"/>
+      <c r="H48" s="11"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
-      <c r="K48" s="13"/>
+      <c r="K48" s="11"/>
       <c r="L48" s="5"/>
       <c r="M48" s="5"/>
-      <c r="N48" s="13"/>
+      <c r="N48" s="11"/>
       <c r="O48" s="5"/>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B49" s="11">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B49" s="10">
         <v>2</v>
       </c>
-      <c r="C49" s="5"/>
+      <c r="C49" s="5">
+        <v>27</v>
+      </c>
       <c r="D49" s="5"/>
-      <c r="E49" s="13">
+      <c r="E49" s="11">
         <v>2</v>
       </c>
-      <c r="F49" s="6"/>
+      <c r="F49" s="6">
+        <v>58</v>
+      </c>
       <c r="G49" s="5"/>
-      <c r="H49" s="13"/>
+      <c r="H49" s="11"/>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
-      <c r="K49" s="13"/>
+      <c r="K49" s="11"/>
       <c r="L49" s="5"/>
       <c r="M49" s="5"/>
-      <c r="N49" s="13"/>
+      <c r="N49" s="11"/>
       <c r="O49" s="5"/>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B50" s="11">
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B50" s="10">
         <v>4</v>
       </c>
-      <c r="C50" s="5"/>
+      <c r="C50" s="5">
+        <v>11.6</v>
+      </c>
       <c r="D50" s="5"/>
-      <c r="E50" s="13">
+      <c r="E50" s="11">
         <v>4</v>
       </c>
-      <c r="F50" s="6"/>
+      <c r="F50" s="6">
+        <v>15</v>
+      </c>
       <c r="G50" s="5"/>
-      <c r="H50" s="13"/>
+      <c r="H50" s="11"/>
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
-      <c r="K50" s="13"/>
+      <c r="K50" s="11"/>
       <c r="L50" s="5"/>
       <c r="M50" s="5"/>
-      <c r="N50" s="13"/>
+      <c r="N50" s="11"/>
       <c r="O50" s="5"/>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B51" s="11">
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B51" s="10">
         <v>8</v>
       </c>
-      <c r="C51" s="5"/>
+      <c r="C51" s="12">
+        <v>9.6999999999999993</v>
+      </c>
       <c r="D51" s="5"/>
-      <c r="E51" s="13">
+      <c r="E51" s="11">
         <v>8</v>
       </c>
-      <c r="F51" s="6"/>
+      <c r="F51" s="6">
+        <v>11.9</v>
+      </c>
       <c r="G51" s="5"/>
-      <c r="H51" s="13"/>
+      <c r="H51" s="11"/>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
-      <c r="K51" s="13"/>
+      <c r="K51" s="11"/>
       <c r="L51" s="5"/>
       <c r="M51" s="5"/>
-      <c r="N51" s="13"/>
+      <c r="N51" s="11"/>
       <c r="O51" s="5"/>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B52" s="15">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B52" s="13">
         <v>16</v>
       </c>
-      <c r="C52" s="5"/>
+      <c r="C52" s="12">
+        <v>4.9000000000000004</v>
+      </c>
       <c r="D52" s="5"/>
-      <c r="E52" s="16">
+      <c r="E52" s="14">
         <v>16</v>
       </c>
-      <c r="F52" s="6"/>
+      <c r="F52" s="6">
+        <v>9.1</v>
+      </c>
       <c r="G52" s="5"/>
-      <c r="H52" s="16"/>
+      <c r="H52" s="14"/>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
-      <c r="K52" s="16"/>
-      <c r="L52" s="14"/>
+      <c r="K52" s="14"/>
+      <c r="L52" s="12"/>
       <c r="M52" s="5"/>
-      <c r="N52" s="16"/>
+      <c r="N52" s="14"/>
       <c r="O52" s="5"/>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53" s="4">
         <v>32</v>
       </c>
-      <c r="C53" s="5"/>
+      <c r="C53" s="12">
+        <v>2.7</v>
+      </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5">
         <v>32</v>
       </c>
-      <c r="F53" s="6"/>
-    </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B54" s="17">
+      <c r="F53" s="6">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B54" s="15">
         <v>64</v>
       </c>
-      <c r="C54" s="8"/>
+      <c r="C54" s="8">
+        <v>3.4</v>
+      </c>
       <c r="D54" s="8"/>
-      <c r="E54" s="18">
+      <c r="E54" s="16">
         <v>64</v>
       </c>
-      <c r="F54" s="9"/>
+      <c r="F54" s="9">
+        <v>6.1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>